<commit_message>
Latest BOM, schematic PDF and PPT of AMT project.
</commit_message>
<xml_diff>
--- a/AMT HALL EFFECT/04_Project Outputs/Rev 2/05_BOM/LMAT_AMT_V2.xlsx
+++ b/AMT HALL EFFECT/04_Project Outputs/Rev 2/05_BOM/LMAT_AMT_V2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\New Volume\Embdes_Final\LUMAX\AMT_Hall_Effect\AMT_20 pin microcontroller\Design\LMAT_AMT_V2 (24-07-2019 17-15-55)\Project Outputs for LMAT_AMT_V2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\New Volume\Embdes_Final\LUMAX\AMT_Hall_Effect\AMT_20 pin microcontroller\Design\Project Outputs for LMAT_AMT_V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="3930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8985"/>
   </bookViews>
   <sheets>
     <sheet name="LMAT_AMT_V2" sheetId="1" r:id="rId1"/>
@@ -278,16 +278,16 @@
     <t>J1</t>
   </si>
   <si>
-    <t>CONN HEADER SMD R/A 8POS 1.27MM</t>
-  </si>
-  <si>
-    <t>Samtec Inc.</t>
-  </si>
-  <si>
-    <t>FTSH-104-02-L-DH</t>
-  </si>
-  <si>
-    <t>SAM11248-ND</t>
+    <t>J-LINK 6-PIN NEEDLE ADAPTER</t>
+  </si>
+  <si>
+    <t>Segger Microcontroller Systems</t>
+  </si>
+  <si>
+    <t>8.06.16 J-LINK 6-PIN NEEDLE ADAPTER</t>
+  </si>
+  <si>
+    <t>899-1051-ND</t>
   </si>
   <si>
     <t>J3</t>
@@ -613,15 +613,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -903,19 +906,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
     <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
@@ -948,7 +950,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -974,7 +976,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1000,7 +1002,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1026,7 +1028,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1052,7 +1054,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1078,7 +1080,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1104,7 +1106,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1130,7 +1132,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1156,7 +1158,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1182,7 +1184,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="4" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1208,7 +1210,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1234,7 +1236,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1260,7 +1262,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="4" t="s">
         <v>79</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1286,7 +1288,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="4" t="s">
         <v>88</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1312,7 +1314,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="4" t="s">
         <v>93</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1338,7 +1340,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="4" t="s">
         <v>98</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1364,7 +1366,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="4" t="s">
         <v>104</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1390,7 +1392,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="4" t="s">
         <v>109</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1416,7 +1418,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
         <v>115</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1442,7 +1444,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="4" t="s">
         <v>120</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1468,7 +1470,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="4" t="s">
         <v>126</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1494,7 +1496,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1520,7 +1522,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="4" t="s">
         <v>136</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1546,7 +1548,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="4" t="s">
         <v>141</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1572,7 +1574,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="4" t="s">
         <v>146</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1598,7 +1600,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="4" t="s">
         <v>152</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1624,7 +1626,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="4" t="s">
         <v>156</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1650,7 +1652,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="4" t="s">
         <v>161</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1676,7 +1678,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="4" t="s">
         <v>165</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -1702,55 +1704,34 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H35" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>12</v>
@@ -1759,24 +1740,24 @@
         <v>13</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="H36" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>53</v>
+      <c r="A37" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>12</v>
@@ -1785,24 +1766,24 @@
         <v>13</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="H37" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>78</v>
+      <c r="A38" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>12</v>
@@ -1811,24 +1792,24 @@
         <v>13</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="H38" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>151</v>
+      <c r="A39" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>147</v>
+        <v>65</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>148</v>
+        <v>67</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>12</v>
@@ -1837,24 +1818,24 @@
         <v>13</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>150</v>
+        <v>68</v>
       </c>
       <c r="H39" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>83</v>
+      <c r="A40" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>84</v>
+        <v>147</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>86</v>
+        <v>148</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>12</v>
@@ -1863,15 +1844,41 @@
         <v>13</v>
       </c>
       <c r="G40" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="H40" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H41" s="3">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C32:E33"/>
+    <mergeCell ref="C32:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
BOM OF VTS_V2 PROJECT
</commit_message>
<xml_diff>
--- a/AMT HALL EFFECT/04_Project Outputs/Rev 2/05_BOM/LMAT_AMT_V2.xlsx
+++ b/AMT HALL EFFECT/04_Project Outputs/Rev 2/05_BOM/LMAT_AMT_V2.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\New Volume\Embdes_Final\LUMAX\AMT_Hall_Effect\Project Outputs for LMAT_AMT_V2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User-1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6255"/>
   </bookViews>
   <sheets>
     <sheet name="LMAT_AMT_V2" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,11 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -623,8 +628,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -660,7 +665,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -672,7 +677,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -689,9 +694,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -719,14 +724,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -754,6 +776,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -908,18 +947,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
     <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1419,25 +1459,25 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>107</v>
+        <v>33</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="H20" s="3">
         <v>1</v>
@@ -1445,25 +1485,25 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>33</v>
+        <v>129</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="H21" s="3">
         <v>1</v>
@@ -1471,103 +1511,103 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="H22" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H23" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="H24" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="H25" s="3">
         <v>1</v>
@@ -1575,25 +1615,25 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H26" s="3">
         <v>1</v>
@@ -1601,25 +1641,25 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="H27" s="3">
         <v>1</v>
@@ -1627,132 +1667,130 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>157</v>
+        <v>122</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>158</v>
+        <v>124</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>158</v>
+        <v>124</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>159</v>
+        <v>125</v>
       </c>
       <c r="H28" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>122</v>
+        <v>162</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>123</v>
+        <v>163</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>124</v>
+        <v>164</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>124</v>
+        <v>164</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>125</v>
+        <v>165</v>
       </c>
       <c r="H29" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>163</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="H30" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="H31" s="3">
         <v>6</v>
       </c>
     </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C32" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D32" s="5"/>
+    </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C33" s="5" t="s">
-        <v>170</v>
-      </c>
+      <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>27</v>
+        <v>117</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>28</v>
+        <v>118</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>115</v>
@@ -1761,24 +1799,24 @@
         <v>13</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>30</v>
+        <v>119</v>
       </c>
       <c r="H37" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>117</v>
+        <v>16</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>118</v>
+        <v>18</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>115</v>
@@ -1787,24 +1825,24 @@
         <v>13</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>119</v>
+        <v>20</v>
       </c>
       <c r="H38" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>16</v>
+        <v>122</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>17</v>
+        <v>123</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>18</v>
+        <v>124</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>115</v>
@@ -1813,24 +1851,24 @@
         <v>13</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>20</v>
+        <v>125</v>
       </c>
       <c r="H39" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>122</v>
+        <v>54</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>123</v>
+        <v>10</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>124</v>
+        <v>55</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>115</v>
@@ -1839,24 +1877,24 @@
         <v>13</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>125</v>
+        <v>57</v>
       </c>
       <c r="H40" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>115</v>
@@ -1865,7 +1903,7 @@
         <v>13</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="H41" s="3">
         <v>1</v>
@@ -1873,7 +1911,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C33:E34"/>
+    <mergeCell ref="C32:D33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>